<commit_message>
Update tong hop danh sach trong cong ty
</commit_message>
<xml_diff>
--- a/QUANGHANH2/excel/TCLD/TongHopNhanSu/Tổng-hợp-nhân-lực.xlsx
+++ b/QUANGHANH2/excel/TCLD/TongHopNhanSu/Tổng-hợp-nhân-lực.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22026"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FA79A44-82CC-483E-99F1-B5A2CC77B0CD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ABE3525-5CEF-4CE8-B9EE-43A21258BEE2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -108,7 +108,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,12 +143,6 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF00B050"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -248,7 +242,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -257,9 +251,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -557,13 +548,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R48"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomRight" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="18.75"/>
@@ -590,43 +581,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" s="2" customFormat="1" ht="20.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="7" t="s">
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="7" t="s">
+      <c r="K1" s="7"/>
+      <c r="L1" s="7"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="5" t="s">
+      <c r="O1" s="7"/>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="4" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:18" s="3" customFormat="1">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
       <c r="D2" s="3" t="s">
         <v>5</v>
       </c>
@@ -669,25 +660,7 @@
       <c r="Q2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="R2" s="6"/>
-    </row>
-    <row r="3" spans="1:18">
-      <c r="A3" s="3"/>
-    </row>
-    <row r="4" spans="1:18">
-      <c r="A4" s="4"/>
-    </row>
-    <row r="21" spans="1:1">
-      <c r="A21" s="4"/>
-    </row>
-    <row r="22" spans="1:1">
-      <c r="A22" s="4"/>
-    </row>
-    <row r="42" spans="1:1">
-      <c r="A42" s="4"/>
-    </row>
-    <row r="48" spans="1:1">
-      <c r="A48" s="4"/>
+      <c r="R2" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>